<commit_message>
added working ImportPointDistributions method, edited the excel import files to match enums, created CreatePointDistribution method in factory
</commit_message>
<xml_diff>
--- a/Data/Excel/TournamentCategoryPoints - Testing.xlsx
+++ b/Data/Excel/TournamentCategoryPoints - Testing.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="20">
   <si>
     <t>Points</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -34,49 +31,49 @@
     <t>ATP-250</t>
   </si>
   <si>
-    <t>Q-1</t>
-  </si>
-  <si>
-    <t>Q-2</t>
-  </si>
-  <si>
-    <t>Q-3</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
-    <t>R-128</t>
-  </si>
-  <si>
-    <t>R-64</t>
-  </si>
-  <si>
-    <t>R-32</t>
-  </si>
-  <si>
-    <t>R-16</t>
-  </si>
-  <si>
-    <t>Quarter Final</t>
-  </si>
-  <si>
-    <t>Semi Final</t>
-  </si>
-  <si>
-    <t>Final</t>
-  </si>
-  <si>
     <t>ATP-500</t>
   </si>
   <si>
-    <t>ATP-Finals</t>
-  </si>
-  <si>
     <t>Grand Slam</t>
   </si>
   <si>
     <t>Masters-1000</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>R128</t>
+  </si>
+  <si>
+    <t>QF</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ATP-Fs</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R16</t>
   </si>
 </sst>
 </file>
@@ -121,9 +118,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,24 +431,25 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -453,41 +457,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -495,27 +499,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -523,13 +527,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -537,13 +541,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -551,13 +555,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D9">
         <v>45</v>
@@ -565,13 +569,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D10">
         <v>90</v>
@@ -579,13 +583,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11">
         <v>150</v>
@@ -593,13 +597,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D12">
         <v>250</v>
@@ -607,83 +611,83 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>250</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>48</v>
       </c>
-      <c r="C15" t="s">
-        <v>14</v>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>90</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
       <c r="D16">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>48</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
-        <v>11</v>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -691,83 +695,83 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
-        <v>8</v>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>32</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -775,27 +779,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B26">
         <v>32</v>
       </c>
-      <c r="C26" t="s">
-        <v>8</v>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -803,27 +807,27 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B27">
         <v>32</v>
       </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B28">
         <v>32</v>
       </c>
-      <c r="C28" t="s">
-        <v>10</v>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -831,13 +835,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B29">
-        <v>32</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -845,13 +849,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B30">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
-        <v>12</v>
+      <c r="C30" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D30">
         <v>45</v>
@@ -859,13 +863,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B31">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>13</v>
+      <c r="C31" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -873,13 +877,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B32">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
-        <v>14</v>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D32">
         <v>180</v>
@@ -887,13 +891,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
-        <v>15</v>
+      <c r="C33" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D33">
         <v>300</v>
@@ -901,13 +905,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
-      <c r="C34" t="s">
-        <v>16</v>
+      <c r="C34" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D34">
         <v>500</v>
@@ -915,83 +919,83 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B35">
         <v>48</v>
       </c>
-      <c r="C35" t="s">
-        <v>16</v>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D35">
-        <v>500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>48</v>
       </c>
-      <c r="C36" t="s">
-        <v>15</v>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D36">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B37">
         <v>48</v>
       </c>
-      <c r="C37" t="s">
-        <v>14</v>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B38">
         <v>48</v>
       </c>
-      <c r="C38" t="s">
-        <v>13</v>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D38">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B39">
         <v>48</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D39">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>48</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B40">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
       </c>
       <c r="D40">
         <v>20</v>
@@ -999,83 +1003,83 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B41">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>1</v>
+      <c r="C41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41">
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>48</v>
       </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1</v>
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B43">
         <v>48</v>
       </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1</v>
+      <c r="C43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B44">
         <v>48</v>
       </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1</v>
+      <c r="C44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44">
+        <v>300</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B45">
         <v>48</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
+      <c r="C45" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>500</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B46">
         <v>8</v>
       </c>
-      <c r="C46" t="s">
-        <v>6</v>
+      <c r="C46" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D46">
         <v>200</v>
@@ -1083,13 +1087,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
-      <c r="C47" t="s">
-        <v>7</v>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D47">
         <v>200</v>
@@ -1097,13 +1101,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48">
         <v>8</v>
       </c>
-      <c r="C48" t="s">
-        <v>8</v>
+      <c r="C48" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D48">
         <v>200</v>
@@ -1111,13 +1115,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B49">
         <v>8</v>
       </c>
-      <c r="C49" t="s">
-        <v>9</v>
+      <c r="C49" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D49">
         <v>200</v>
@@ -1125,13 +1129,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
-        <v>10</v>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D50">
         <v>200</v>
@@ -1139,13 +1143,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>8</v>
       </c>
-      <c r="C51" t="s">
-        <v>11</v>
+      <c r="C51" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D51">
         <v>200</v>
@@ -1153,13 +1157,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B52">
-        <v>8</v>
-      </c>
-      <c r="C52" t="s">
-        <v>12</v>
       </c>
       <c r="D52">
         <v>200</v>
@@ -1167,13 +1171,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>8</v>
       </c>
-      <c r="C53" t="s">
-        <v>13</v>
+      <c r="C53" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D53">
         <v>200</v>
@@ -1181,13 +1185,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
-      <c r="C54" t="s">
-        <v>14</v>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D54">
         <v>600</v>
@@ -1195,13 +1199,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B55">
         <v>8</v>
       </c>
-      <c r="C55" t="s">
-        <v>15</v>
+      <c r="C55" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D55">
         <v>1000</v>
@@ -1209,13 +1213,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56">
         <v>8</v>
       </c>
-      <c r="C56" t="s">
-        <v>16</v>
+      <c r="C56" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D56">
         <v>1500</v>
@@ -1223,83 +1227,83 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B57">
         <v>128</v>
       </c>
-      <c r="C57" t="s">
-        <v>16</v>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D57">
-        <v>2000</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>128</v>
       </c>
-      <c r="C58" t="s">
-        <v>15</v>
+      <c r="C58" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>1200</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B59">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
-        <v>14</v>
+      <c r="C59" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>720</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B60">
         <v>128</v>
       </c>
-      <c r="C60" t="s">
-        <v>13</v>
+      <c r="C60" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D60">
-        <v>360</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B61">
         <v>128</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D61">
-        <v>180</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <v>128</v>
       </c>
-      <c r="C62" t="s">
-        <v>11</v>
+      <c r="C62" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D62">
         <v>90</v>
@@ -1307,139 +1311,139 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B63">
         <v>128</v>
       </c>
-      <c r="C63" t="s">
-        <v>10</v>
+      <c r="C63" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D63">
-        <v>45</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>128</v>
       </c>
-      <c r="C64" t="s">
-        <v>9</v>
+      <c r="C64" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>360</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B65">
         <v>128</v>
       </c>
-      <c r="C65" t="s">
-        <v>8</v>
+      <c r="C65" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D65">
-        <v>25</v>
+        <v>720</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B66">
         <v>128</v>
       </c>
-      <c r="C66" t="s">
-        <v>7</v>
+      <c r="C66" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D66">
-        <v>16</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>128</v>
       </c>
-      <c r="C67" t="s">
-        <v>6</v>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D67">
-        <v>8</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B68">
         <v>56</v>
       </c>
-      <c r="C68" t="s">
-        <v>8</v>
+      <c r="C68" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D68">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B69">
         <v>56</v>
       </c>
-      <c r="C69" t="s">
-        <v>6</v>
+      <c r="C69" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B70">
         <v>56</v>
       </c>
-      <c r="C70" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1</v>
+      <c r="C70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B71">
         <v>56</v>
       </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" t="s">
-        <v>1</v>
+      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B72">
         <v>56</v>
       </c>
-      <c r="C72" t="s">
-        <v>10</v>
+      <c r="C72" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -1447,13 +1451,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B73">
         <v>56</v>
       </c>
-      <c r="C73" t="s">
-        <v>11</v>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D73">
         <v>45</v>
@@ -1461,13 +1465,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B74">
         <v>56</v>
       </c>
-      <c r="C74" t="s">
-        <v>12</v>
+      <c r="C74" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D74">
         <v>90</v>
@@ -1475,13 +1479,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B75">
         <v>56</v>
       </c>
-      <c r="C75" t="s">
-        <v>13</v>
+      <c r="C75" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D75">
         <v>180</v>
@@ -1489,125 +1493,125 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B76">
         <v>56</v>
       </c>
-      <c r="C76" t="s">
-        <v>16</v>
+      <c r="C76" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D76">
-        <v>1000</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B77">
         <v>56</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D77">
-        <v>360</v>
+        <v>600</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B78">
         <v>56</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D78">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B79">
         <v>96</v>
       </c>
-      <c r="C79" t="s">
-        <v>15</v>
+      <c r="C79" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D79">
-        <v>600</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B80">
         <v>96</v>
       </c>
-      <c r="C80" t="s">
-        <v>14</v>
+      <c r="C80" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D80">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B81">
         <v>96</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81">
         <v>16</v>
-      </c>
-      <c r="D81">
-        <v>1000</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B82">
         <v>96</v>
       </c>
-      <c r="C82" t="s">
-        <v>13</v>
+      <c r="C82" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D82">
-        <v>180</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B83">
         <v>96</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D83">
-        <v>90</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B84">
         <v>96</v>
       </c>
-      <c r="C84" t="s">
-        <v>11</v>
+      <c r="C84" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D84">
         <v>45</v>
@@ -1615,72 +1619,72 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B85">
         <v>96</v>
       </c>
-      <c r="C85" t="s">
-        <v>10</v>
+      <c r="C85" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D85">
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B86">
         <v>96</v>
       </c>
-      <c r="C86" t="s">
-        <v>9</v>
+      <c r="C86" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B87">
         <v>96</v>
       </c>
-      <c r="C87" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1</v>
+      <c r="C87" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>360</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B88">
         <v>96</v>
       </c>
-      <c r="C88" t="s">
-        <v>6</v>
+      <c r="C88" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D88">
-        <v>16</v>
+        <v>600</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B89">
         <v>96</v>
       </c>
-      <c r="C89" t="s">
-        <v>8</v>
+      <c r="C89" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D89">
-        <v>16</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>